<commit_message>
Atualizando as métricas e a navbar da página do BobIa
</commit_message>
<xml_diff>
--- a/entregaveis-grupo/documentacao/metricas.xlsx
+++ b/entregaveis-grupo/documentacao/metricas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usúario\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Documents\FACULDADE\SPRINT2\WineTech\entregaveis-grupo\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8F4C40-7CE4-492D-A65C-3B1431215DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03167B8D-3885-47A7-90C0-94F26A7DD890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E0EEE3D4-0ED8-4755-84A3-B19FB26DA5D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E0EEE3D4-0ED8-4755-84A3-B19FB26DA5D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,15 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="40">
   <si>
     <t>Barril</t>
   </si>
@@ -109,18 +112,6 @@
     <t>Crítico</t>
   </si>
   <si>
-    <t>60%  -  50%</t>
-  </si>
-  <si>
-    <t>70%  -  80%</t>
-  </si>
-  <si>
-    <t>80%  -  90%</t>
-  </si>
-  <si>
-    <t>50%  -  40%</t>
-  </si>
-  <si>
     <t>Legenda</t>
   </si>
   <si>
@@ -139,10 +130,46 @@
     <t>19°C  -  21°C</t>
   </si>
   <si>
-    <t>22°C  -  25°C</t>
-  </si>
-  <si>
-    <t>6°C  - -5°C</t>
+    <t xml:space="preserve">-5°C  -  6°C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 80% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 50% </t>
+  </si>
+  <si>
+    <t>TEMPERATURA</t>
+  </si>
+  <si>
+    <t>UMIDADE</t>
+  </si>
+  <si>
+    <t>&lt; -5°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 21°C  </t>
+  </si>
+  <si>
+    <t>50%  -  59%</t>
+  </si>
+  <si>
+    <t>71%  -  80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crítico </t>
+  </si>
+  <si>
+    <t>Moderada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crítica </t>
+  </si>
+  <si>
+    <t>CENÁRIO TEMPERATURA IDEAL</t>
+  </si>
+  <si>
+    <t>CENÁRIO UMIDADE IDEAL</t>
   </si>
 </sst>
 </file>
@@ -161,13 +188,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="30"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,6 +222,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -246,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -269,41 +297,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425B9E49-6ABD-49F8-8F59-9555333EDC6E}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,145 +753,445 @@
     <col min="3" max="3" width="17.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" ht="43.2" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="E1"/>
+      <c r="F1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2"/>
+      <c r="F2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="J3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="D6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="F9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="L9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C11" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="F14" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="10" t="s">
+    </row>
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="F15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G2:H2"/>
+  <mergeCells count="7">
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>